<commit_message>
emails alunos projeto intermediario
</commit_message>
<xml_diff>
--- a/projeto_intermediario.xlsx
+++ b/projeto_intermediario.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Alunos</t>
   </si>
@@ -42,15 +42,24 @@
     <t xml:space="preserve">AWS DeepRace</t>
   </si>
   <si>
+    <t>felipemcd@al.insper.edu.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">HUDSON MONTEIRO</t>
   </si>
   <si>
     <t xml:space="preserve">JOÃO ALONSO CASELLA</t>
   </si>
   <si>
+    <t>j.casella2002@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">JOÃO GABRIEL VALENTIM ROCHA</t>
   </si>
   <si>
+    <t>Valentim@neroai.com.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">JOÃO LUCAS DE MORAES BARROS CADORNIGA</t>
   </si>
   <si>
@@ -60,9 +69,15 @@
     <t xml:space="preserve">LUIZ FELIPE LAZZARON</t>
   </si>
   <si>
+    <t>luizfl@al.insper.edu.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marcelo Rabello Barranco</t>
   </si>
   <si>
+    <t>rabello.barranco@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">MARCOS PAULO RICARTE REBOUÇAS</t>
   </si>
   <si>
@@ -78,14 +93,20 @@
     <t xml:space="preserve">RODRIGO ANCIÃES PATELLI</t>
   </si>
   <si>
+    <t>rodrigoap8@al.insper.edu.br</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOMAS RODRIGUES ALESSI</t>
+  </si>
+  <si>
+    <t>tomasalessi@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -104,6 +125,12 @@
       <sz val="10.500000"/>
       <color rgb="FF262626"/>
       <name val="Open Sans"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,12 +153,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,31 +724,40 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" ht="15.75">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" ht="15.75">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" ht="15.75">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" ht="15.75">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -728,7 +765,7 @@
     </row>
     <row r="11" ht="15.75">
       <c r="A11" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -736,23 +773,29 @@
     </row>
     <row r="12" ht="15.75">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" ht="15.75">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
+      <c r="D13" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" ht="15.75">
       <c r="A14" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
@@ -760,7 +803,7 @@
     </row>
     <row r="15" ht="15.75">
       <c r="A15" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -768,7 +811,7 @@
     </row>
     <row r="16" ht="15.75">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -776,7 +819,7 @@
     </row>
     <row r="17" ht="15.75">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>2</v>
@@ -784,18 +827,24 @@
     </row>
     <row r="18" ht="15.75">
       <c r="A18" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
+      <c r="D18" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" ht="15.75">
       <c r="A19" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="14.25"/>
@@ -935,6 +984,15 @@
     <row r="154" ht="14.25"/>
     <row r="155" ht="14.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D6"/>
+    <hyperlink r:id="rId2" ref="D8"/>
+    <hyperlink r:id="rId3" ref="D9"/>
+    <hyperlink r:id="rId4" ref="D12"/>
+    <hyperlink r:id="rId5" ref="D13"/>
+    <hyperlink r:id="rId6" ref="D18"/>
+    <hyperlink r:id="rId7" ref="D19"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>

</xml_diff>